<commit_message>
implement CalculatePage+ update pom file
</commit_message>
<xml_diff>
--- a/Documents/HMM_Requirements.xlsx
+++ b/Documents/HMM_Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">HMM </t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Grap the type of bill in pie chart</t>
+  </si>
+  <si>
+    <t>Sent email to Users in home about detail paid</t>
   </si>
 </sst>
 </file>
@@ -115,8 +118,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -414,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,8 +542,12 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>

</xml_diff>